<commit_message>
Updated BAT and added PM
</commit_message>
<xml_diff>
--- a/BAT.xlsx
+++ b/BAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konst\iCloudDrive\Documents\valuations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9544CF91-FC76-4AE1-B29E-37C5E6E520D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47C7B5B-E794-46E5-A80A-87CC9FAB632A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="767" activeTab="5" xr2:uid="{A454576F-BA0E-4C95-85A1-1E0F525C6E61}"/>
+    <workbookView xWindow="5985" yWindow="3195" windowWidth="38700" windowHeight="15345" tabRatio="767" activeTab="5" xr2:uid="{A454576F-BA0E-4C95-85A1-1E0F525C6E61}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -21,9 +21,6 @@
     <sheet name="Historical" sheetId="10" r:id="rId6"/>
     <sheet name="INPUT&gt;&gt;" sheetId="6" r:id="rId7"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId8"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -611,7 +608,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -695,7 +692,6 @@
     <xf numFmtId="15" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -740,49 +736,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Cover"/>
-      <sheetName val="Manual"/>
-      <sheetName val="Disclaimer"/>
-      <sheetName val="Input"/>
-      <sheetName val="WORKINGS&gt;&gt;"/>
-      <sheetName val="Valuation"/>
-      <sheetName val="Model"/>
-      <sheetName val="Historical"/>
-      <sheetName val="INPUT&gt;&gt;"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3">
-        <row r="8">
-          <cell r="E8" t="str">
-            <v>BHP</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="E14" t="str">
-            <v>USDmn</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1469,7 +1422,7 @@
   <dimension ref="A1:AA734"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -1512,8 +1465,8 @@
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.2">
       <c r="E8" s="5" t="str">
-        <f>Input!$E$8&amp;" P&amp;L"</f>
-        <v>BAT P&amp;L</v>
+        <f>Input!$E$8&amp;" - P&amp;L"</f>
+        <v>BAT - P&amp;L</v>
       </c>
       <c r="O8" s="9"/>
       <c r="Q8" s="34" t="s">
@@ -1857,20 +1810,20 @@
       <c r="E21" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="45"/>
-      <c r="L21" s="45"/>
-      <c r="M21" s="45">
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16">
         <v>-1641</v>
       </c>
-      <c r="N21" s="45">
+      <c r="N21" s="16">
         <v>-1895</v>
       </c>
-      <c r="O21" s="45">
+      <c r="O21" s="16">
         <v>-1098</v>
       </c>
       <c r="Q21" s="35" t="str">
@@ -2215,16 +2168,16 @@
     </row>
     <row r="37" spans="3:27" x14ac:dyDescent="0.2">
       <c r="E37" s="5" t="str">
-        <f>[1]Input!$E$8&amp;" BS"</f>
-        <v>BHP BS</v>
+        <f>Input!$E$8&amp;" - BS"</f>
+        <v>BAT - BS</v>
       </c>
       <c r="O37" s="9"/>
       <c r="AA37" s="30"/>
     </row>
     <row r="38" spans="3:27" x14ac:dyDescent="0.2">
       <c r="E38" s="10" t="str">
-        <f>+[1]Input!$E$14</f>
-        <v>USDmn</v>
+        <f>+Input!$E$14</f>
+        <v>£m</v>
       </c>
       <c r="F38" s="21"/>
       <c r="G38" s="21"/>

</xml_diff>